<commit_message>
sending refactor output of schedule for doctor
</commit_message>
<xml_diff>
--- a/workers/current_schedule.xlsx
+++ b/workers/current_schedule.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26219"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26220"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFE25454-25B4-4B93-98AF-0CBDC7AA30A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE054C17-3610-4BF4-BB9D-09B776FB3E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -625,7 +625,7 @@
   <dimension ref="A1:BC20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -756,7 +756,7 @@
     </row>
     <row r="2" spans="1:55">
       <c r="A2" s="8">
-        <v>44983</v>
+        <v>44984</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
admin deferred schedule beta function add
</commit_message>
<xml_diff>
--- a/workers/current_schedule.xlsx
+++ b/workers/current_schedule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26220"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4112FAB5-DD3A-40AE-983B-817EDA74679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{279F3596-9426-42EA-BC06-16456E09D03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Инструкция по пользованию" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="35">
   <si>
     <t>Важная информация</t>
   </si>
@@ -132,12 +132,6 @@
   </si>
   <si>
     <t>Боба</t>
-  </si>
-  <si>
-    <t>asjdfasjkdfkjasdkfj;alsdkfj;lasdjfas;lfjdslfjasl;fdfjlksa;djfasl;kjdf;laksjdflasjfasl;kf;laksdf</t>
-  </si>
-  <si>
-    <t>Boba2asd</t>
   </si>
   <si>
     <t>Boba2</t>
@@ -462,21 +456,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -497,36 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,111 +845,111 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1"/>
     <row r="6" spans="1:14" ht="15" customHeight="1">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="32"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="17"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="B8" s="12"/>
@@ -973,189 +967,189 @@
       <c r="N8" s="12"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="24"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1"/>
     <row r="14" spans="1:14" ht="15" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="27"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="22"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="26"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="18"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="28"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="18"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="28"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="18"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="28"/>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="18"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="28"/>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="21"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="31"/>
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1"/>
     <row r="22" spans="1:14" ht="15" customHeight="1"/>
@@ -1211,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7710581-9497-4FBA-B909-8BE874C91BC1}">
   <dimension ref="A1:BC20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1581,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC17DE14-1C8B-4E6F-B36A-0458C238EC85}">
   <dimension ref="A1:BC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -1713,49 +1707,49 @@
     </row>
     <row r="2" spans="1:55">
       <c r="A2" s="8">
-        <v>44983</v>
+        <v>44985</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="8">
         <f>A2+1</f>
-        <v>44984</v>
+        <v>44986</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q2" s="8">
         <f>A2+2</f>
-        <v>44985</v>
+        <v>44987</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Y2" s="8">
         <f>A2+3</f>
-        <v>44986</v>
+        <v>44988</v>
       </c>
       <c r="Z2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="AG2" s="8">
         <f>A2+4</f>
-        <v>44987</v>
+        <v>44989</v>
       </c>
       <c r="AH2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="AO2" s="8">
         <f>A2+5</f>
-        <v>44988</v>
+        <v>44990</v>
       </c>
       <c r="AP2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="AW2" s="8">
         <f>A2+6</f>
-        <v>44989</v>
+        <v>44991</v>
       </c>
       <c r="AX2" s="7" t="s">
         <v>17</v>
@@ -1976,24 +1970,6 @@
       <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="2">
-        <v>678678</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="AX6" s="11">
         <v>0.75</v>
       </c>
@@ -2027,7 +2003,7 @@
         <v>678678</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>